<commit_message>
sydw Signed-off-by: fengjinliang <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/sydw/2020上/考点/思想.xlsx
+++ b/sydw/2020上/考点/思想.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20175" windowHeight="11670"/>
+    <workbookView windowWidth="19200" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="中国特色社会主义理论体系" sheetId="1" r:id="rId1"/>
     <sheet name="毛泽东思想" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="马克思主义" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>一个中心，两个基本点</t>
   </si>
@@ -100,6 +100,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国特色社会主义道路</t>
     </r>
     <r>
@@ -138,6 +145,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国特色社会主义理论体系</t>
     </r>
     <r>
@@ -173,6 +187,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国特色社会主义制度</t>
     </r>
     <r>
@@ -208,6 +229,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国特色社会主义文化</t>
     </r>
     <r>
@@ -352,10 +380,46 @@
     <t>三个代表是我们党保持先进性、始终成为建设有中国社会主义坚强领导核心的基本要求</t>
   </si>
   <si>
+    <t>改革是坚持和发展中国特色社会主义的必由之路，他的性质是一场伟大革命。</t>
+  </si>
+  <si>
+    <t>改革</t>
+  </si>
+  <si>
+    <t>我国的改革不是对原有体制作细枝末节的修补，而是对原有体制的根本性改革。</t>
+  </si>
+  <si>
+    <t>改革开放</t>
+  </si>
+  <si>
+    <t>改革是从根本上改变束缚生产力发展的经济、政治和其他领域的改革，而非仅仅是对生产(经济)的改革。</t>
+  </si>
+  <si>
+    <t>改革是对已经建立的社会主义制度的巩固、发展和完善</t>
+  </si>
+  <si>
+    <t>改革是对社会主义制度中不适应社会生产力的发展部分进行革新和改变，以达到适应生产力发展需求的目的。</t>
+  </si>
+  <si>
+    <t>这是社会主义制度框架下对社会制度的自我完善、自我发展、并没有改变社会主义制度的性质，不是对社会主义基本制度的变革。</t>
+  </si>
+  <si>
+    <t>16.4会</t>
+  </si>
+  <si>
+    <t>科学执政(前提)、民主执政(本质)、依法执政(途径)三者相互联系、有机结合，构成了我党执政方式的基本理论框架</t>
+  </si>
+  <si>
     <t>灵魂</t>
   </si>
   <si>
     <t>实事求是、群众路线、独立自主</t>
+  </si>
+  <si>
+    <t>1956年对农业、手工业、资本主义工商业的社会主义改造基本完成。标准我国几千年的阶级剥削结束，实现了由新民主主义向社会主义社会的转变，社会主义基本制度在我国初步建立</t>
+  </si>
+  <si>
+    <t>马克思主义哲学</t>
   </si>
 </sst>
 </file>
@@ -365,10 +429,10 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,37 +442,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -420,6 +456,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -428,8 +471,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,7 +578,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,83 +591,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -544,187 +601,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,6 +792,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -753,30 +819,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -788,6 +830,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -821,17 +878,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -840,148 +897,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -989,13 +1046,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1346,13 +1403,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C5:L75"/>
+  <dimension ref="C5:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="5" spans="3:12">
       <c r="C5" s="1" t="s">
@@ -1650,6 +1707,50 @@
     <row r="75" spans="6:6">
       <c r="F75" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6">
+      <c r="F79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="5:6">
+      <c r="E80" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6">
+      <c r="C81" t="s">
+        <v>75</v>
+      </c>
+      <c r="F81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6">
+      <c r="F82" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="6:6">
+      <c r="F83" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="6:6">
+      <c r="F84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6">
+      <c r="D86" t="s">
+        <v>80</v>
+      </c>
+      <c r="F86" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1662,20 +1763,25 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="E6:F6"/>
+  <dimension ref="E6:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <sheetData>
     <row r="6" spans="5:6">
       <c r="E6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1688,14 +1794,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="3" spans="4:4">
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>